<commit_message>
exercise 3 of set 2 completed
</commit_message>
<xml_diff>
--- a/set2/my-excel.xlsx
+++ b/set2/my-excel.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="4920"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="lala" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>this is my excel</t>
+  </si>
+  <si>
+    <t>values</t>
   </si>
 </sst>
 </file>
@@ -357,15 +360,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>